<commit_message>
Error of the first table fixed
</commit_message>
<xml_diff>
--- a/1toolConverter_local/parametros.xlsx
+++ b/1toolConverter_local/parametros.xlsx
@@ -10,7 +10,6 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tabla_1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tabla_2" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tabla_3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tabla_4" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,61 +427,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Author</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Keyter - Departamento de Control</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ESKEYM03AU</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Application</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7984,7 +7928,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -15741,7 +15685,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Interfaz funcional, problemas con la tabla, notis y clasificacion
</commit_message>
<xml_diff>
--- a/1toolConverter_local/parametros.xlsx
+++ b/1toolConverter_local/parametros.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Parametros_Unificados" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Parametros_Unificados" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>